<commit_message>
solucion para algunos nos encontrados
</commit_message>
<xml_diff>
--- a/empresas.xlsx
+++ b/empresas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Programas sin finalizar\ScrapingSUNAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CF5B2B-3713-441A-AEEA-788B947C4CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DDD0A4-542E-493B-8783-5D2E4BC70CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4B4C5AA1-E11C-494E-965B-EC1DE9B609BF}"/>
   </bookViews>
@@ -37,48 +37,609 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="201">
   <si>
     <t>razon_social</t>
   </si>
   <si>
-    <t>SOFIA LIBRERIA Y BAZAR SOCIEDAD COMERCIAL DE RESPONSABILIDAD LIMITADA</t>
-  </si>
-  <si>
-    <t>SPECIAL BOOK SERVICES S.A.</t>
-  </si>
-  <si>
-    <t>SYT COMPANY S.A.C.</t>
-  </si>
-  <si>
-    <t>TATI Y DEYANIRA LIBRERIA BAZAR S.R.L.</t>
-  </si>
-  <si>
-    <t>TONINA E.I.R.L.</t>
-  </si>
-  <si>
-    <t>UNIVERSO EMPRESARIAL S.A.C.</t>
-  </si>
-  <si>
-    <t>UTILES &amp; MAS LIBRERÍA BAZAR E.I.R.L.</t>
-  </si>
-  <si>
-    <t>VH FERRETERIA &amp; LIBRERIA SOCIEDAD COMERCIAL DE RESPONSABILIDAD LIMITADA - VH FERRETERIA &amp; LIBRERIA S</t>
-  </si>
-  <si>
-    <t>VQ IMPORTACIONES PERU S.A.C.</t>
-  </si>
-  <si>
-    <t>WALAH LIBRERIAS E.I.R.L.</t>
-  </si>
-  <si>
-    <t>WINNAAR MV S.R.L.</t>
-  </si>
-  <si>
-    <t>YOKOTA INVERSIONES S.A.C.</t>
-  </si>
-  <si>
-    <t>YOVIS C &amp; M LIBRERIA Y ACCESORIOS E.I.R.L.</t>
+    <t>NOVATE S.A.P S.A.C.</t>
+  </si>
+  <si>
+    <t>OM E HIJOS REPRESENTACIONES S.A.C.</t>
+  </si>
+  <si>
+    <t>ORIGINAL KOREA IMPORT E.I.R.L.</t>
+  </si>
+  <si>
+    <t>OSAN MOTORS S.A.C.</t>
+  </si>
+  <si>
+    <t>PARABRISAS DELIVERY LIMA S.A.C.</t>
+  </si>
+  <si>
+    <t>PERU MASTER AUTOMOCION Y SERVICIOS S.A.C.</t>
+  </si>
+  <si>
+    <t>PERU TODO 4 X 4 S.A.C.</t>
+  </si>
+  <si>
+    <t>PETRI CORP S.A.C.</t>
+  </si>
+  <si>
+    <t>PRAIG SOLUTIONS S.A.C.</t>
+  </si>
+  <si>
+    <t>PREVEN SERVICIOS E.I.R.L.</t>
+  </si>
+  <si>
+    <t>PROTEMAX S.A.C.</t>
+  </si>
+  <si>
+    <t>PROTIRES &amp; CAR BOUTIQUE E.I.R.L.</t>
+  </si>
+  <si>
+    <t>PROVEEDORA LOGISTICA S.A.C.</t>
+  </si>
+  <si>
+    <t>QINGDAO TYRES PERU S.A.C.</t>
+  </si>
+  <si>
+    <t>R.A Y N.J FERCAT CORPORACION E.I.R.L.</t>
+  </si>
+  <si>
+    <t>RADIADORES BARRETO SRL</t>
+  </si>
+  <si>
+    <t>RADIADORES FREELINE S.R.L.</t>
+  </si>
+  <si>
+    <t>RED DINAMO S.A.C.</t>
+  </si>
+  <si>
+    <t>RENTA CAR WALLACE E.I.R.L.</t>
+  </si>
+  <si>
+    <t>REPRESENTACIONES MJV E.I.R.L</t>
+  </si>
+  <si>
+    <t>REPUESTOS JAPONESES S.A.</t>
+  </si>
+  <si>
+    <t>RG - HYDRO E.I.R.L</t>
+  </si>
+  <si>
+    <t>RJ HOLDING PERU SOCIEDAD ANONIMA CERRADA</t>
+  </si>
+  <si>
+    <t>RODASIA AUTO PARTS S.A.C</t>
+  </si>
+  <si>
+    <t>ROMA IMPORT PERU S.A.C.</t>
+  </si>
+  <si>
+    <t>S &amp; C CONTINENTAL PACIFICO E.I.R.L.</t>
+  </si>
+  <si>
+    <t>S &amp; M IMPORTADORES S.A.C.</t>
+  </si>
+  <si>
+    <t>S.J.DISTRIBUCIONES S.A.C.</t>
+  </si>
+  <si>
+    <t>SAILING POINT S.A.C.</t>
+  </si>
+  <si>
+    <t>SAKANA IMPORT EMPRESA INDIVIDUAL DE RESPONSABILIDAD LIMITAD</t>
+  </si>
+  <si>
+    <t>SALES WAR S.A.C.</t>
+  </si>
+  <si>
+    <t>SAMI KAY PERU E.I.R.L.</t>
+  </si>
+  <si>
+    <t>SANJEQ CORPORATION S.A.C.</t>
+  </si>
+  <si>
+    <t>SERV TECN DEL AIRE PA LA IND LA MIN SA</t>
+  </si>
+  <si>
+    <t>SERVICEMAQ AMSE E.I.R.L.</t>
+  </si>
+  <si>
+    <t>SERVICENTRO VIRGEN DE CHAPI SOCIEDAD ANONIMA CERRADA</t>
+  </si>
+  <si>
+    <t>SERVICIOS GENERALES KORIAKI E.I.R.L.</t>
+  </si>
+  <si>
+    <t>SERVICIOS LOGISTICOS DIESEL S.A.C. - SLD S.A.C.</t>
+  </si>
+  <si>
+    <t>SLOT CASINO SELVA S.A.C.</t>
+  </si>
+  <si>
+    <t>SMF PERUANA SOCIEDAD ANONIMA CERRADA</t>
+  </si>
+  <si>
+    <t>SOBRE 4 RUEDAS E.I.R.L.</t>
+  </si>
+  <si>
+    <t>SOLUCIONES MEDICAS TECNOLOGICAS E.I.R.L.</t>
+  </si>
+  <si>
+    <t>SOPORTES DE VEHICULOS Y EXTINTORES FELIX E.I.R.L.</t>
+  </si>
+  <si>
+    <t>SOUTH HORIZON SOCIEDAD ANONIMA CERRADA</t>
+  </si>
+  <si>
+    <t>SOUTH TIRES PERU SOCIEDAD ANONIMA CERRADA - SOUTH TIRES S.A.C.</t>
+  </si>
+  <si>
+    <t>SPEED-PERU SOCIEDAD ANONIMA CERRADA</t>
+  </si>
+  <si>
+    <t>SPIN PERU S.A.C.</t>
+  </si>
+  <si>
+    <t>SUPPLIES &amp; MAINTENANCE SERVICES SAC</t>
+  </si>
+  <si>
+    <t>TALLER AUTOGAS PERU S.A.C.</t>
+  </si>
+  <si>
+    <t>TORO TRADE COMPANY E.I.R.L.</t>
+  </si>
+  <si>
+    <t>TORQUE S.A.C.</t>
+  </si>
+  <si>
+    <t>TOTAL 4X4 BUSINESS S.A.C.</t>
+  </si>
+  <si>
+    <t>TOTAL MOTORING S.A.C.</t>
+  </si>
+  <si>
+    <t>TRACTOPARTES-VR E.I.R.L.</t>
+  </si>
+  <si>
+    <t>TRADE SERVICE A &amp; E S.A.C.</t>
+  </si>
+  <si>
+    <t>VALLE ALTO MAQUINARIAS E.I.R.L.</t>
+  </si>
+  <si>
+    <t>VELOTAXI UNO S.A.C.</t>
+  </si>
+  <si>
+    <t>VENTAS MINERIA BARRICK PERU E.I.R.L.</t>
+  </si>
+  <si>
+    <t>WAREHOUSE PARTS E.I.R.L. - W.PARTS E.I.R.L.</t>
+  </si>
+  <si>
+    <t>WICE SERVICIOS CORPORATIVOS S.A.C.</t>
+  </si>
+  <si>
+    <t>ZULFROOTS S.R.L</t>
+  </si>
+  <si>
+    <t>25 AM E.I.R.L.</t>
+  </si>
+  <si>
+    <t>2JZ AUTOMOTIVE SAC</t>
+  </si>
+  <si>
+    <t>A &amp; V REPUESTOS SAN ANDRES S.A.C.</t>
+  </si>
+  <si>
+    <t>ABBA OIL COMPANY S.A.C.</t>
+  </si>
+  <si>
+    <t>AC.STAG S.A.C.</t>
+  </si>
+  <si>
+    <t>ACCESORIOS MEZA E.I.R.L.</t>
+  </si>
+  <si>
+    <t>ALFREDO PIMENTEL SEVILLA S A</t>
+  </si>
+  <si>
+    <t>ALL ASIAN MOTORS E.I.R.L.</t>
+  </si>
+  <si>
+    <t>ALROMA TOOLS PERU S.A.C.</t>
+  </si>
+  <si>
+    <t>AMERICAN CAR SYSTEM S.A.C.</t>
+  </si>
+  <si>
+    <t>AQP MOTOR PART E.I.R.L</t>
+  </si>
+  <si>
+    <t>ASCHIERO VENTAS E.I.R.L.</t>
+  </si>
+  <si>
+    <t>ASESORIA Y REPARACION DE AUTOS Y MOTORES SOCIEDAD ANONIMA CERRADA</t>
+  </si>
+  <si>
+    <t>ASPEN CAPITAL S.A.C. - ASPENCA S.A.C.</t>
+  </si>
+  <si>
+    <t>AUTO BOUTIQUE FL S.A.C.</t>
+  </si>
+  <si>
+    <t>AUTO BOUTIQUE ML. E.I.R.L.</t>
+  </si>
+  <si>
+    <t>AUTO PARTS ELECTRICAL F &amp; N S.A.C.</t>
+  </si>
+  <si>
+    <t>AUTO PARTS ELECTRICAL FERNANDO E.I.R.L.</t>
+  </si>
+  <si>
+    <t>AUTO SPORT ARAMBURU E.I.R.L.</t>
+  </si>
+  <si>
+    <t>AUTO TUNING CHINA-USA IMPORT S.A.C.</t>
+  </si>
+  <si>
+    <t>AUTODISA REPUESTOS E.I.R.L.</t>
+  </si>
+  <si>
+    <t>AUTOMOTRIZ MARIMON S.A.C.</t>
+  </si>
+  <si>
+    <t>AUTOPARTES Y ACCESORIOS ZUPER PRIME MOTOR'S S.R.L.</t>
+  </si>
+  <si>
+    <t>AUTOREPUESTOS Y SERVICIOS C J E.I.R.L.</t>
+  </si>
+  <si>
+    <t>AUTORUS PERU E.I.R.L.</t>
+  </si>
+  <si>
+    <t>AUTOS MOTORPARTS E.I.R.L.</t>
+  </si>
+  <si>
+    <t>AUTOS MOTORVOL S.A.C.</t>
+  </si>
+  <si>
+    <t>AUTOTECHNIK S.A.C.</t>
+  </si>
+  <si>
+    <t>AUTOZENTRUM SERVICIOS AUTOMOTRICES S.A.C.</t>
+  </si>
+  <si>
+    <t>BLANK' IT E.I.R.L.</t>
+  </si>
+  <si>
+    <t>BRAKE SOLUTION E.I.R.L.</t>
+  </si>
+  <si>
+    <t>BRANNETT PERU E.I.R.L.</t>
+  </si>
+  <si>
+    <t>CADEC MAQUINARIAS SOCIEDAD ANONIMA CERRADA</t>
+  </si>
+  <si>
+    <t>CARBURADORES KOKOLISO IMPORT E.I.R.L.</t>
+  </si>
+  <si>
+    <t>CARPLAY S.A.C.</t>
+  </si>
+  <si>
+    <t>CAUTIVO MUFFLER SHOP E.I.R.L.</t>
+  </si>
+  <si>
+    <t>CDF AUTOMOTRIZ S.A.C.</t>
+  </si>
+  <si>
+    <t>CHINCHA 4X4 STORE S.A.C.</t>
+  </si>
+  <si>
+    <t>CLEVER CAPITAL SOCIEDAD ANONIMA CERRADA</t>
+  </si>
+  <si>
+    <t>COLD TECHNOLOGY PERU S.A.C.</t>
+  </si>
+  <si>
+    <t>COMERCIALIZADORA DE REPUESTOS &amp; SUMINISTROS LA MEJOR S.R.L.</t>
+  </si>
+  <si>
+    <t>COMERCIO AUTOMOTRIZ S.A.C.</t>
+  </si>
+  <si>
+    <t>CORDOVA SERVICE PERU E.I.R.L.</t>
+  </si>
+  <si>
+    <t>CORPORACION DECOVA S.A.C.</t>
+  </si>
+  <si>
+    <t>CORPORACION INZ.COM S.A.C.</t>
+  </si>
+  <si>
+    <t>CORPORACION JOFRAN F&amp;S S.A.C.</t>
+  </si>
+  <si>
+    <t>CORPORACION JOFRAN-CLAUSTE E.I.R.L.</t>
+  </si>
+  <si>
+    <t>CORPORACION MAGIC VAS E.I.R.L.</t>
+  </si>
+  <si>
+    <t>CORPORACION WBU DE REPUESTOS Y SERVICIOS E.I.R.L.</t>
+  </si>
+  <si>
+    <t>CORPORACION Z1 SOCIEDAD ANONIMA CERRADA - CORPORACION Z1 S.A.C.</t>
+  </si>
+  <si>
+    <t>CORPORACION Z1 SUR SOCIEDAD ANONIMA CERRADA</t>
+  </si>
+  <si>
+    <t>CRISTAL FILMS S.A.C.</t>
+  </si>
+  <si>
+    <t>CRISTALES EXPRESS LIMA S.A.C.</t>
+  </si>
+  <si>
+    <t>DAKAL SERVICE BRAKES E.I.R.L.</t>
+  </si>
+  <si>
+    <t>DELTA PERU SOCIEDAD ANONIMA CERRADA</t>
+  </si>
+  <si>
+    <t>DEMA S A</t>
+  </si>
+  <si>
+    <t>DIPCAR.PE S.A.C.</t>
+  </si>
+  <si>
+    <t>DISTRIBUCION E IMPORTACIONES DE REPUESTOS EUROPEOS Y AMERICANOS S.A.C.</t>
+  </si>
+  <si>
+    <t>DISTRIBUCIONES TECNICAS S.A.C.</t>
+  </si>
+  <si>
+    <t>DISTRIBUIDORA DE REPUESTOS ANDINOS E.I.R.L.</t>
+  </si>
+  <si>
+    <t>DISTRIBUIDORA DE REPUESTOS AUTOMOTRICES INDUSTRIALES S.A.C. - DRAI S.A.C.</t>
+  </si>
+  <si>
+    <t>DISTRIBUIDORA VEGA S A</t>
+  </si>
+  <si>
+    <t>EDWIN CAR TUNING SERVICE S.A.C.</t>
+  </si>
+  <si>
+    <t>EL REFUGIO DEL RIDER E.I.R.L.</t>
+  </si>
+  <si>
+    <t>ELECTRICAL PARTS FLORES S.A.C.</t>
+  </si>
+  <si>
+    <t>ELEGANT CARS PERU E.I.R.L- ELEGAN CARS</t>
+  </si>
+  <si>
+    <t>EUROMARCAS S.A.C.</t>
+  </si>
+  <si>
+    <t>EVOLUTION NEW CARS SAC</t>
+  </si>
+  <si>
+    <t>F &amp; D IMPORT SOCIEDAD ANONIMA CERRADA</t>
+  </si>
+  <si>
+    <t>F &amp; E RONDINEL E.I.R.L.</t>
+  </si>
+  <si>
+    <t>FALCONELLO S.A.C.</t>
+  </si>
+  <si>
+    <t>FILTROCENTRO PERU E.I.R.L.</t>
+  </si>
+  <si>
+    <t>G &amp; C INVERSIONES Y NEGOCIOS S.A.C.</t>
+  </si>
+  <si>
+    <t>GARAGE 1640 S.A.C.</t>
+  </si>
+  <si>
+    <t>GB2 SOLUTIONS S.A.C.</t>
+  </si>
+  <si>
+    <t>GNC PARTES S.A.C.</t>
+  </si>
+  <si>
+    <t>GOLD TRACK &amp; CIA S.R.L.</t>
+  </si>
+  <si>
+    <t>GR PERFOMANCE &amp; SERVICE SOCIEDAD COMERCIAL DE RESPONSABILIDAD LIMITADA</t>
+  </si>
+  <si>
+    <t>GRUPO AUTOMOTRIZ DE VEHÍCULOS DE ALTA GAMA S.A.C.</t>
+  </si>
+  <si>
+    <t>HEAD AUTOBOUTIQUE E.I.R.L.</t>
+  </si>
+  <si>
+    <t>HERRAMIENTAS Y MANGUERAS FERNANDO ALONSO E.I.R.L</t>
+  </si>
+  <si>
+    <t>IMPORTACION Y DISTRIBUCION DE REPUESTOS AUTOMOTRIZ ANDINOS E.I.R.L.</t>
+  </si>
+  <si>
+    <t>IMPORTACION Y DISTRIBUCION DE REPUESTOS F &amp; D E.I.R.L.</t>
+  </si>
+  <si>
+    <t>IMPORTACIONES CMC EIRL</t>
+  </si>
+  <si>
+    <t>IMPORTACIONES LAZART S.A.C.</t>
+  </si>
+  <si>
+    <t>IMPORTACIONES ORMAVI SOCIEDAD ANONIMA CERRADA - ORMAVI S.A.C.</t>
+  </si>
+  <si>
+    <t>IMPORTACIONES SAN MIGUEL S.A.C.</t>
+  </si>
+  <si>
+    <t>IMPORTACIONES Y SERVICIOS PYD S.A.C.</t>
+  </si>
+  <si>
+    <t>IMPORTADORA DE AUTOPARTES ANDINOS S.A.C.</t>
+  </si>
+  <si>
+    <t>IMPORTADORA DE REPUESTOS AL TOKE S.A.C.</t>
+  </si>
+  <si>
+    <t>IMPORTADORA DE REPUESTOS PERU S.A.C.</t>
+  </si>
+  <si>
+    <t>IMPORTADORA SATERI EIRL</t>
+  </si>
+  <si>
+    <t>INDUBAT E.I.R.L.</t>
+  </si>
+  <si>
+    <t>INDUSTRIAS MORA S.A.C.</t>
+  </si>
+  <si>
+    <t>INNOVACIONES LYD E.I.R.L.</t>
+  </si>
+  <si>
+    <t>INVERSION LI IMPORT &amp; EXPORT S.A.C</t>
+  </si>
+  <si>
+    <t>INVERSIONES BRANIC S.A.C.</t>
+  </si>
+  <si>
+    <t>INVERSIONES GOLDEN CARS S.A.C.</t>
+  </si>
+  <si>
+    <t>INVERSIONES IMPORTADORA &amp; EXPORTADORA FALUCO E.I.R.L.</t>
+  </si>
+  <si>
+    <t>INVERSIONES LEON X&amp;S S.A.C</t>
+  </si>
+  <si>
+    <t>INVERSIONES MUÑOZ SEGURA &amp; HNOS E.I.R.L.</t>
+  </si>
+  <si>
+    <t>J &amp; J POWER PERU IMPORT EXPORT E.I.R.L.</t>
+  </si>
+  <si>
+    <t>J.CH.COMERCIAL S.A.</t>
+  </si>
+  <si>
+    <t>JB MANGUERAS &amp; REPUESTOS E.I.R.L.</t>
+  </si>
+  <si>
+    <t>JEBES ECERF EMPRESA INDIVIDUAL DE RESPONSABILIDAD LIMITADA - JEBES ECERF E.I.R.L.</t>
+  </si>
+  <si>
+    <t>JOSSIMPORT PERU E.I.R.L.</t>
+  </si>
+  <si>
+    <t>KING FILTERS PERU S.A.C.</t>
+  </si>
+  <si>
+    <t>KING PARTS HONDA S.A.C.</t>
+  </si>
+  <si>
+    <t>LA CALERA SERVICIOS GENERALES S.A.C.</t>
+  </si>
+  <si>
+    <t>LAM HP SERVICIOS GENERALES E.I.R.L.</t>
+  </si>
+  <si>
+    <t>LIMATAMBO CAR SERVICE S.A.</t>
+  </si>
+  <si>
+    <t>LLANTAMIGO S.A.C.</t>
+  </si>
+  <si>
+    <t>LUBRICANTES D`CARLOS E.I.R.L.</t>
+  </si>
+  <si>
+    <t>LUBRICANTES INKA MOTORS INDIVIDUAL DE RESPONSABILIDAD LIMITADA - LIBRICANTES INKA MOTORS E.I.R.L.</t>
+  </si>
+  <si>
+    <t>LUBRIMAX S.A</t>
+  </si>
+  <si>
+    <t>M &amp; M APPLIANCE PARTS S.R.L.</t>
+  </si>
+  <si>
+    <t>M&amp;G AUTOMOTIVE SOCIEDAD ANÓNIMA CERRADA</t>
+  </si>
+  <si>
+    <t>M.M.M. CUEVA IMPORT &amp; EXPORT E.I.R.L.</t>
+  </si>
+  <si>
+    <t>M/R AUTODESIGN E.I.R.L.</t>
+  </si>
+  <si>
+    <t>MAPISA CORPORATION S.A.C.</t>
+  </si>
+  <si>
+    <t>MC TECNOLOGY S.A.C.</t>
+  </si>
+  <si>
+    <t>MECANICA AUTOMOTRIZ J CHINO E.I.R.L.</t>
+  </si>
+  <si>
+    <t>MIAMI PARTS PERU S.A.C.</t>
+  </si>
+  <si>
+    <t>MORA AUTOMOTRIZ &amp; ASOCIADOS S.A.C.</t>
+  </si>
+  <si>
+    <t>MOTORARED S.A.C.</t>
+  </si>
+  <si>
+    <t>MULTIMARCAS ANEXAS EN GRADO E.I.R.L.</t>
+  </si>
+  <si>
+    <t>MULTISERVICIOS E INGENIERIA M &amp; N S.A.C.</t>
+  </si>
+  <si>
+    <t>MY SUPER AUTO S.A.C.</t>
+  </si>
+  <si>
+    <t>NEWGAS IMPORT S.A.C.</t>
+  </si>
+  <si>
+    <t>ORO DIESEL PERU S.A.C.</t>
+  </si>
+  <si>
+    <t>PANGU (PERU) NEW ENERGY VEHICLE SALES S.A.C.</t>
+  </si>
+  <si>
+    <t>PARTS SHOP IMPORT E.I.R.L.</t>
+  </si>
+  <si>
+    <t>PERNOS &amp; TUERCAS ANGAMOS E.I.R.L.</t>
+  </si>
+  <si>
+    <t>PORTSSHING COMPANY S.A.C.</t>
+  </si>
+  <si>
+    <t>PROMAX TRADE IMPORT SOCIEDAD ANONIMA CERRADA</t>
+  </si>
+  <si>
+    <t>QUISWAR S.A.C.</t>
+  </si>
+  <si>
+    <t>R A REPUESTOS ORIGINALES S.A.C.</t>
+  </si>
+  <si>
+    <t>RACING BRAND S.A.C.</t>
+  </si>
+  <si>
+    <t>RADIADORES D &amp; M IMPORT E.I.R.L.</t>
   </si>
 </sst>
 </file>
@@ -451,10 +1012,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F5111E-E63C-42FC-90AA-352ED2BE978B}">
-  <dimension ref="B1:B151"/>
+  <dimension ref="B1:B201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B14"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,12 +1028,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:2" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -482,7 +1043,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -493,7 +1054,7 @@
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -502,7 +1063,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="2:2" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
@@ -527,421 +1088,945 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="2:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="17" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="18" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="19" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="20" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="1"/>
+      <c r="B20" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="21" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="2"/>
+      <c r="B21" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="22" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="23" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="1"/>
+      <c r="B23" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="24" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="1"/>
+      <c r="B24" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="25" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="26" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="1"/>
+      <c r="B26" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="27" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="1"/>
+      <c r="B27" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="28" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="1"/>
+      <c r="B28" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="29" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="2"/>
+      <c r="B29" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="30" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="1"/>
+      <c r="B30" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="31" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="1"/>
+      <c r="B31" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="32" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="1"/>
+      <c r="B32" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="33" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="1"/>
+      <c r="B33" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="34" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="1"/>
+      <c r="B34" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="35" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="1"/>
+      <c r="B35" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="36" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="1"/>
+      <c r="B36" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="37" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="1"/>
-    </row>
-    <row r="38" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="1"/>
+      <c r="B37" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="39" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="1"/>
+      <c r="B39" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="40" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="1"/>
+      <c r="B40" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="41" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="1"/>
+      <c r="B41" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="42" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="1"/>
+      <c r="B42" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="43" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="1"/>
+      <c r="B43" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="44" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="1"/>
+      <c r="B44" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="45" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="1"/>
+      <c r="B45" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="46" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="1"/>
+      <c r="B46" s="2" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="47" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="1"/>
+      <c r="B47" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="48" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="1"/>
+      <c r="B48" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="49" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="1"/>
+      <c r="B49" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="50" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="1"/>
+      <c r="B50" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="51" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="1"/>
+      <c r="B51" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="52" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="1"/>
+      <c r="B52" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="53" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="1"/>
+      <c r="B53" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="54" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="2"/>
+      <c r="B54" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="55" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="1"/>
+      <c r="B55" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="56" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="1"/>
+      <c r="B56" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="57" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="2"/>
+      <c r="B57" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="58" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="1"/>
-    </row>
-    <row r="59" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="2"/>
+      <c r="B58" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="1" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="60" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="1"/>
-    </row>
-    <row r="61" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="1"/>
+      <c r="B60" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="1" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="62" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="2"/>
+      <c r="B62" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="63" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="2"/>
+      <c r="B63" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="64" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="1"/>
+      <c r="B64" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="65" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="1"/>
+      <c r="B65" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="66" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="1"/>
+      <c r="B66" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="67" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="1"/>
+      <c r="B67" s="1" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="68" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="1"/>
+      <c r="B68" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="69" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="1"/>
+      <c r="B69" s="1" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="70" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="2"/>
+      <c r="B70" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="71" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="2"/>
+      <c r="B71" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="72" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="1"/>
+      <c r="B72" s="1" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="73" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="2"/>
+      <c r="B73" s="1" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="74" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="2"/>
+      <c r="B74" s="1" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="75" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="1"/>
-    </row>
-    <row r="76" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="1"/>
+      <c r="B75" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="1" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="77" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="1"/>
+      <c r="B77" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="78" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="1"/>
+      <c r="B78" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="79" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="1"/>
+      <c r="B79" s="1" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="80" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="1"/>
+      <c r="B80" s="2" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="81" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="1"/>
+      <c r="B81" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="82" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="1"/>
+      <c r="B82" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="83" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="1"/>
+      <c r="B83" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="84" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="1"/>
+      <c r="B84" s="1" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="85" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="1"/>
-    </row>
-    <row r="86" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="1"/>
+      <c r="B85" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B86" s="1" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="87" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="2"/>
+      <c r="B87" s="1" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="88" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="1"/>
+      <c r="B88" s="1" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="89" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="1"/>
+      <c r="B89" s="1" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="90" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="1"/>
+      <c r="B90" s="1" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="91" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="1"/>
+      <c r="B91" s="2" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="92" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="2"/>
+      <c r="B92" s="1" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="93" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="1"/>
+      <c r="B93" s="1" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="94" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="2"/>
+      <c r="B94" s="1" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="95" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="1"/>
+      <c r="B95" s="2" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="96" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="2"/>
+      <c r="B96" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="97" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="1"/>
+      <c r="B97" s="1" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="98" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="1"/>
+      <c r="B98" s="1" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="99" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="1"/>
+      <c r="B99" s="1" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="100" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="1"/>
+      <c r="B100" s="1" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="101" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="1"/>
+      <c r="B101" s="2" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="102" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="1"/>
+      <c r="B102" s="1" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="103" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="1"/>
+      <c r="B103" s="2" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="104" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="1"/>
+      <c r="B104" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="105" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B105" s="1"/>
+      <c r="B105" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="106" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="2"/>
+      <c r="B106" s="1" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="107" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B107" s="1"/>
+      <c r="B107" s="1" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="108" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="1"/>
-    </row>
-    <row r="109" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B109" s="2"/>
+      <c r="B108" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B109" s="1" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="110" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B110" s="1"/>
+      <c r="B110" s="1" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="111" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B111" s="2"/>
+      <c r="B111" s="2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="112" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B112" s="1"/>
+      <c r="B112" s="2" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="113" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B113" s="2"/>
+      <c r="B113" s="2" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="114" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B114" s="1"/>
+      <c r="B114" s="1" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="115" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B115" s="1"/>
+      <c r="B115" s="1" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="116" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B116" s="1"/>
+      <c r="B116" s="1" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="117" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B117" s="1"/>
+      <c r="B117" s="2" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="118" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B118" s="1"/>
+      <c r="B118" s="1" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="119" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B119" s="1"/>
+      <c r="B119" s="1" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="120" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B120" s="2"/>
+      <c r="B120" s="2" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="121" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="2"/>
+      <c r="B121" s="1" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="122" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B122" s="1"/>
+      <c r="B122" s="2" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="123" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B123" s="1"/>
+      <c r="B123" s="2" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="124" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B124" s="1"/>
+      <c r="B124" s="1" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="125" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B125" s="1"/>
+      <c r="B125" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="126" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B126" s="1"/>
+      <c r="B126" s="1" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="127" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B127" s="2"/>
+      <c r="B127" s="1" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="128" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B128" s="2"/>
+      <c r="B128" s="2" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="129" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B129" s="2"/>
+      <c r="B129" s="1" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="130" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B130" s="1"/>
+      <c r="B130" s="1" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="131" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B131" s="1"/>
+      <c r="B131" s="2" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="132" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B132" s="1"/>
+      <c r="B132" s="1" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="133" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B133" s="1"/>
+      <c r="B133" s="1" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="134" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B134" s="1"/>
-    </row>
-    <row r="135" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B135" s="1"/>
+      <c r="B134" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135" spans="2:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B135" s="1" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="136" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B136" s="1"/>
+      <c r="B136" s="1" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="137" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B137" s="1"/>
+      <c r="B137" s="1" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="138" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B138" s="2"/>
+      <c r="B138" s="1" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="139" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B139" s="1"/>
+      <c r="B139" s="1" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="140" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B140" s="1"/>
+      <c r="B140" s="2" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="141" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B141" s="1"/>
+      <c r="B141" s="2" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="142" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B142" s="1"/>
+      <c r="B142" s="1" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="143" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B143" s="1"/>
+      <c r="B143" s="2" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="144" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B144" s="1"/>
+      <c r="B144" s="2" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="145" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B145" s="1"/>
+      <c r="B145" s="2" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="146" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B146" s="1"/>
+      <c r="B146" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="147" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B147" s="1"/>
+      <c r="B147" s="1" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="148" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B148" s="1"/>
+      <c r="B148" s="2" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="149" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B149" s="1"/>
-    </row>
-    <row r="150" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B150" s="1"/>
+      <c r="B149" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="150" spans="2:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B150" s="1" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="151" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B151" s="1"/>
+      <c r="B151" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="152" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B152" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="153" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B153" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="154" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B154" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="155" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B155" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="156" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B156" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="157" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B157" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="158" spans="2:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B158" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="159" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B159" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="160" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B160" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="161" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B161" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="162" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B162" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="163" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B163" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="164" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B164" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="165" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B165" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="166" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B166" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="167" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B167" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="168" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B168" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="169" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B169" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="170" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B170" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="171" spans="2:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B171" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="172" spans="2:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B172" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="173" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B173" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="174" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B174" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="175" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B175" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="176" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B176" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="177" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B177" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="178" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B178" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="179" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B179" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="180" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B180" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="181" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B181" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="182" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B182" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="183" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B183" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="184" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B184" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="185" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B185" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="186" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B186" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="187" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B187" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="188" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B188" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="189" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B189" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="190" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B190" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="191" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B191" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="192" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B192" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="193" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B193" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="194" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B194" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="195" spans="2:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B195" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="196" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B196" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="197" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B197" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="198" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B198" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="199" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B199" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="200" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B200" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="201" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B201" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>